<commit_message>
Colonists Are Not Zergling小人可不是小狗 (1.5) 추가(fix)
(일부 가독성을 위해 수정)
</commit_message>
<xml_diff>
--- a/Pull Request Here/Colonists Are Not Zergling小人可不是小狗 (1.5) - 3250618949/Colonists Are Not Zergling小人可不是小狗 (1.5) - 3250618949.xlsx
+++ b/Pull Request Here/Colonists Are Not Zergling小人可不是小狗 (1.5) - 3250618949/Colonists Are Not Zergling小人可不是小狗 (1.5) - 3250618949.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PDSSO2\Desktop\RimworldExtractor-Standard\RIM EXCEL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF0A580C-AB45-4BA8-8A27-ADBD1D20E2AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{938CB3E1-A605-4CFD-B6A1-3BEA0BF500E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -113,10 +113,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>기념비 최대 크기 (최소 3)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>임무에 필요한 정착민 최대 수</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -134,6 +130,10 @@
   </si>
   <si>
     <t>임무에 필요한 정착민 수를 계산할 때 아래의 배율을 곱하여 결정합니다.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>기념비의 비석 최대 개수 (최소 3)</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -536,7 +536,7 @@
         <v>25</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -550,10 +550,10 @@
         <v>10</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -604,7 +604,7 @@
         <v>18</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
@@ -621,7 +621,7 @@
         <v>21</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
@@ -638,7 +638,7 @@
         <v>24</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>